<commit_message>
feat: tambah sales dan referral (import lead)
</commit_message>
<xml_diff>
--- a/public/assets/template/excel/lead_sample.xlsx
+++ b/public/assets/template/excel/lead_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My PC\Documents\ITTP\skripsi\cazh_crm\public\assets\template\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2381BE8B-394A-484E-BE61-5CADD5E7D857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AECA10-6F2E-4514-A4B1-87276FD863A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{02C6D976-823C-42EC-9A77-A7CAE796E8F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{02C6D976-823C-42EC-9A77-A7CAE796E8F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>PIC Partner</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>Lembaga</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Hari</t>
+  </si>
+  <si>
+    <t>Imam</t>
+  </si>
+  <si>
+    <t>Dita</t>
+  </si>
+  <si>
+    <t>Referral</t>
   </si>
 </sst>
 </file>
@@ -124,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -161,6 +176,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABBBD2-F3B7-4CEE-AB28-64477D4F7101}">
-  <dimension ref="A1:E238"/>
+  <dimension ref="A1:G238"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="E4" sqref="A4:E4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -486,10 +507,11 @@
     <col min="1" max="2" width="34.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="5"/>
+    <col min="5" max="5" width="13.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -505,8 +527,14 @@
       <c r="E1" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -522,8 +550,14 @@
       <c r="E2" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -539,92 +573,98 @@
       <c r="E3" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="9"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="10"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="9"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="9"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="9"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="9"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="9"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="9"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="9"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="9"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:7">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2192,21 +2232,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050935D35F384AF4BBC451617A5CE5789" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="36129ec10bbeef0e9ea748d7e210619b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21072794-4655-4b81-b930-2614394ba3c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74da23e7bf6ab3e31fda5cf45c033a6a" ns3:_="">
     <xsd:import namespace="21072794-4655-4b81-b930-2614394ba3c3"/>
@@ -2344,7 +2369,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC1EB740-B332-40DB-8E7F-DF8A1F0FDAE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="21072794-4655-4b81-b930-2614394ba3c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3A76C18-4B3C-42B6-8028-D29B20A02B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2360,28 +2418,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFED54D6-58BC-423A-A79D-6A043179B50C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC1EB740-B332-40DB-8E7F-DF8A1F0FDAE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="21072794-4655-4b81-b930-2614394ba3c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: update template import (lead)
</commit_message>
<xml_diff>
--- a/public/assets/template/excel/lead_sample.xlsx
+++ b/public/assets/template/excel/lead_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My PC\Documents\ITTP\skripsi\cazh_crm\public\assets\template\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AECA10-6F2E-4514-A4B1-87276FD863A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B09160CB-1F27-4B96-A8C3-9F1D6A41CA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{02C6D976-823C-42EC-9A77-A7CAE796E8F6}"/>
   </bookViews>
@@ -498,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABBBD2-F3B7-4CEE-AB28-64477D4F7101}">
   <dimension ref="A1:G238"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="106" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -2232,6 +2232,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050935D35F384AF4BBC451617A5CE5789" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="36129ec10bbeef0e9ea748d7e210619b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21072794-4655-4b81-b930-2614394ba3c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74da23e7bf6ab3e31fda5cf45c033a6a" ns3:_="">
     <xsd:import namespace="21072794-4655-4b81-b930-2614394ba3c3"/>
@@ -2369,35 +2384,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC1EB740-B332-40DB-8E7F-DF8A1F0FDAE7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFED54D6-58BC-423A-A79D-6A043179B50C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="21072794-4655-4b81-b930-2614394ba3c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2419,9 +2409,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFED54D6-58BC-423A-A79D-6A043179B50C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC1EB740-B332-40DB-8E7F-DF8A1F0FDAE7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="21072794-4655-4b81-b930-2614394ba3c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>